<commit_message>
Integreated new AUT. Added code to highlight element. Added code to take screenshot.
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
+++ b/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="openBrowser" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Browser</t>
   </si>
@@ -33,13 +33,16 @@
     <t>firefox</t>
   </si>
   <si>
-    <t>demo123</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>http://demosite.center/wordpress/wp-login.php</t>
+    <t>http://newtours.demoaut.com/</t>
+  </si>
+  <si>
+    <t>mercury</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Welcome: Mercury Tours</t>
   </si>
 </sst>
 </file>
@@ -392,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +416,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -428,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,14 +457,11 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Android@123"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -463,13 +471,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,14 +492,11 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Android@123"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added class mercuryFlightBooking, dataProvider.
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
+++ b/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="openBrowser" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="inputLoginDetails" sheetId="4" r:id="rId3"/>
-    <sheet name="verifyEnteredValues" sheetId="1" r:id="rId4"/>
-    <sheet name="RegisterNewUser" sheetId="6" r:id="rId5"/>
+    <sheet name="inputLoginDetails" sheetId="4" r:id="rId2"/>
+    <sheet name="verifyEnteredValues" sheetId="1" r:id="rId3"/>
+    <sheet name="RegisterNewUser" sheetId="6" r:id="rId4"/>
+    <sheet name="inputFlightDetails" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Browser</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
     <t>http://newtours.demoaut.com/</t>
   </si>
   <si>
@@ -105,6 +102,57 @@
   </si>
   <si>
     <t>NORWAY</t>
+  </si>
+  <si>
+    <t>Journey Type</t>
+  </si>
+  <si>
+    <t>Round Trip</t>
+  </si>
+  <si>
+    <t>Number of Passengers</t>
+  </si>
+  <si>
+    <t>Departing From</t>
+  </si>
+  <si>
+    <t>Departure Month</t>
+  </si>
+  <si>
+    <t>Departure Day</t>
+  </si>
+  <si>
+    <t>Arriving At</t>
+  </si>
+  <si>
+    <t>Arrival Month</t>
+  </si>
+  <si>
+    <t>Arrival Day</t>
+  </si>
+  <si>
+    <t>Service Class</t>
+  </si>
+  <si>
+    <t>Airline</t>
+  </si>
+  <si>
+    <t>Acapulco</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>Business Class</t>
+  </si>
+  <si>
+    <t>Blue Skies Airlines</t>
+  </si>
+  <si>
+    <t>opera</t>
   </si>
 </sst>
 </file>
@@ -459,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +518,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,15 +526,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -498,18 +546,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -524,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +568,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -559,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -567,7 +603,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -575,11 +611,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -587,23 +623,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>33433243</v>
@@ -611,47 +647,47 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>445544</v>
@@ -659,18 +695,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -678,15 +714,15 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -698,4 +734,100 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added selectFlight, bookFlight function
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
+++ b/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="openBrowser" sheetId="2" r:id="rId1"/>
-    <sheet name="inputLoginDetails" sheetId="4" r:id="rId2"/>
-    <sheet name="verifyEnteredValues" sheetId="1" r:id="rId3"/>
-    <sheet name="RegisterNewUser" sheetId="6" r:id="rId4"/>
-    <sheet name="inputFlightDetails" sheetId="7" r:id="rId5"/>
+    <sheet name="selectFlight" sheetId="8" r:id="rId2"/>
+    <sheet name="bookFlight" sheetId="9" r:id="rId3"/>
+    <sheet name="inputLoginDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="verifyEnteredValues" sheetId="1" r:id="rId5"/>
+    <sheet name="RegisterNewUser" sheetId="6" r:id="rId6"/>
+    <sheet name="inputFlightDetails" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>Browser</t>
   </si>
@@ -153,6 +155,24 @@
   </si>
   <si>
     <t>opera</t>
+  </si>
+  <si>
+    <t>Departure Flight</t>
+  </si>
+  <si>
+    <t>Pangaea Airlines 362</t>
+  </si>
+  <si>
+    <t>Return Flight</t>
+  </si>
+  <si>
+    <t>Unified Airlines 633</t>
+  </si>
+  <si>
+    <t>Departure</t>
+  </si>
+  <si>
+    <t>Arrival</t>
   </si>
 </sst>
 </file>
@@ -507,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -546,6 +566,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -576,7 +690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -611,7 +725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -736,11 +850,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Almost code complete. Need to put logging and comments for furnishing.
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
+++ b/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
   <si>
     <t>Browser</t>
   </si>
@@ -179,6 +179,89 @@
   </si>
   <si>
     <t>Blue Skies Airlines 361</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meal </t>
+  </si>
+  <si>
+    <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>Card Type</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expiry Month </t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>Expiry Year</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Ticketless Travel</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Billing Address 1</t>
+  </si>
+  <si>
+    <t>Billing Address 2</t>
+  </si>
+  <si>
+    <t>Auckland</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Delivery same as billing</t>
+  </si>
+  <si>
+    <t>Delivery Address1</t>
+  </si>
+  <si>
+    <t>Delivery Addrss2</t>
+  </si>
+  <si>
+    <t>1234 5678 9874 1523</t>
+  </si>
+  <si>
+    <t>NEW ZEALAND</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have chosen a mailing location outside of the United States and its territories. An additional charge of $6.5 will be added as mailing charge.
+You have chosen a mailing location outside of the United States and its territories. An additional charge of $6.5 will be added as mailing charge.
+</t>
   </si>
 </sst>
 </file>
@@ -223,9 +306,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -620,10 +707,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,8 +775,209 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23">
+        <v>335443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30">
+        <v>335443</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Logout and closeBrowser code.
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
+++ b/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="openBrowser" sheetId="2" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>Blue Skies Airlines</t>
   </si>
   <si>
-    <t>opera</t>
-  </si>
-  <si>
     <t>Departure Flight</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
     <t xml:space="preserve">You have chosen a mailing location outside of the United States and its territories. An additional charge of $6.5 will be added as mailing charge.
 You have chosen a mailing location outside of the United States and its territories. An additional charge of $6.5 will be added as mailing charge.
 </t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>39</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
@@ -686,18 +686,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -709,19 +709,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>39</v>
@@ -729,7 +729,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
@@ -737,15 +737,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>271</v>
@@ -753,15 +753,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>303</v>
@@ -777,55 +777,55 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
         <v>55</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>2000</v>
@@ -833,39 +833,39 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
         <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -884,7 +884,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -892,12 +892,12 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23">
         <v>335443</v>
@@ -908,20 +908,20 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
         <v>16</v>
@@ -940,7 +940,7 @@
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -948,12 +948,12 @@
         <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30">
         <v>335443</v>
@@ -964,15 +964,15 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1023,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added current URL validation. Documentation is in progress.
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
+++ b/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="openBrowser" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Browser</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>pageURL</t>
+  </si>
+  <si>
+    <t>http://newtours.demoaut.com/create_account_success.php</t>
   </si>
 </sst>
 </file>
@@ -620,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1049,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,14 +1167,23 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B12" r:id="rId2"/>
     <hyperlink ref="B13" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added email functionality :-)
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
+++ b/CertificationProject-HybridFramework/framework/InputData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="openBrowser" sheetId="2" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="verifyEnteredValues" sheetId="1" r:id="rId5"/>
     <sheet name="RegisterNewUser" sheetId="6" r:id="rId6"/>
     <sheet name="inputFlightDetails" sheetId="7" r:id="rId7"/>
+    <sheet name="emailData" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="88">
   <si>
     <t>Browser</t>
   </si>
@@ -268,6 +269,24 @@
   </si>
   <si>
     <t>http://newtours.demoaut.com/create_account_success.php</t>
+  </si>
+  <si>
+    <t>admin email</t>
+  </si>
+  <si>
+    <t>admin pass</t>
+  </si>
+  <si>
+    <t>To addresses</t>
+  </si>
+  <si>
+    <t>admin@gmail.com</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>recipient@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -624,15 +643,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -640,15 +657,16 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1057,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1283,4 +1301,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>